<commit_message>
Update Import & Export Staff
- adding trim for several column
- change download template
- add several validation
</commit_message>
<xml_diff>
--- a/public/template/Template_Input_Staff.xlsx
+++ b/public/template/Template_Input_Staff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadmukhtar/Projects/rpc-be/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49336E6A-C736-9F47-9DF7-1D3DCBA7ADA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075C8985-7C08-3845-86F4-2E8DD9C722B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detail" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="Data Lokasi" sheetId="6" r:id="rId8"/>
     <sheet name="Data Durasi Pembayaran" sheetId="10" r:id="rId9"/>
     <sheet name="Data Kartu Identitas" sheetId="7" r:id="rId10"/>
-    <sheet name="Data Provinsi" sheetId="11" r:id="rId11"/>
-    <sheet name="Data Kabupaten" sheetId="12" r:id="rId12"/>
+    <sheet name="Data Grup Keamanan" sheetId="13" r:id="rId11"/>
+    <sheet name="Data Provinsi" sheetId="11" r:id="rId12"/>
+    <sheet name="Data Kabupaten" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Wajib diisi berdasarkan nomor urut dan tidak boleh duplikat</t>
   </si>
@@ -145,9 +146,6 @@
     <t>Diisi dengan angka 1 atau 0, 1 menandakan ya, 0 menandakan tidak</t>
   </si>
   <si>
-    <t>Pilih Salah satu: Administrator, Manager, Staff, Customer, Internship, Office, dan Doctor</t>
-  </si>
-  <si>
     <t>Pelanggan dapat menjadwalkan anggota staff ini secara online</t>
   </si>
   <si>
@@ -227,6 +225,9 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Diisi menggunakan ID dari sheet Data Grup Keamanan</t>
   </si>
 </sst>
 </file>
@@ -308,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,6 +335,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,7 +635,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -717,7 +723,7 @@
         <v>30</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="119" x14ac:dyDescent="0.2">
@@ -770,7 +776,7 @@
       <c r="Q2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -796,7 +802,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -805,6 +811,30 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA889ADE-68AC-F04D-8AE7-41B9C936F5DB}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B35"/>
   <sheetViews>
@@ -818,10 +848,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -965,7 +995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:C515"/>
   <sheetViews>
@@ -980,13 +1010,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3568,7 +3598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3586,22 +3616,22 @@
         <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -3623,8 +3653,8 @@
       <c r="F2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>33</v>
+      <c r="G2" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3654,22 +3684,22 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -3680,7 +3710,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3704,13 +3734,13 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3718,10 +3748,10 @@
         <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3745,10 +3775,10 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -3756,7 +3786,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -4101,13 +4131,13 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -4115,7 +4145,7 @@
         <v>31</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4163,10 +4193,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing Import & Template Staff
</commit_message>
<xml_diff>
--- a/public/template/Template_Input_Staff.xlsx
+++ b/public/template/Template_Input_Staff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadmukhtar/Projects/rpc-be/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075C8985-7C08-3845-86F4-2E8DD9C722B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BC0642-E392-D648-BAB7-8A4F07F14CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detail" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,9 @@
     <sheet name="Data Grup Keamanan" sheetId="13" r:id="rId11"/>
     <sheet name="Data Provinsi" sheetId="11" r:id="rId12"/>
     <sheet name="Data Kabupaten" sheetId="12" r:id="rId13"/>
+    <sheet name="Data Kegunaan" sheetId="16" r:id="rId14"/>
+    <sheet name="Data Tipe Telepon" sheetId="15" r:id="rId15"/>
+    <sheet name="Data Tipe Messenger" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>Wajib diisi berdasarkan nomor urut dan tidak boleh duplikat</t>
   </si>
@@ -185,27 +188,9 @@
     <t>Jadikan Sebagai Alamat Utama</t>
   </si>
   <si>
-    <t>Diisi Utama atau Cadangan</t>
-  </si>
-  <si>
-    <t>pilihan antara Rumah atau Whatsapp</t>
-  </si>
-  <si>
-    <t>Pemakaian</t>
-  </si>
-  <si>
-    <t>Nomor</t>
-  </si>
-  <si>
-    <t>Tipe</t>
-  </si>
-  <si>
     <t>Alamat Email</t>
   </si>
   <si>
-    <t>Disi angka 1 saja</t>
-  </si>
-  <si>
     <t>Nama Pengguna</t>
   </si>
   <si>
@@ -228,6 +213,39 @@
   </si>
   <si>
     <t>Diisi menggunakan ID dari sheet Data Grup Keamanan</t>
+  </si>
+  <si>
+    <t>ID Pemakaian</t>
+  </si>
+  <si>
+    <t>Nomor Telepon</t>
+  </si>
+  <si>
+    <t>ID Tipe</t>
+  </si>
+  <si>
+    <t>Wajib diisi menggunakan ID Pemakaian yang ada di sheet Data Pemakaian</t>
+  </si>
+  <si>
+    <t>Wajib diisi menggunakan ID Tipe yang ada di sheet Data Tipe Telepon</t>
+  </si>
+  <si>
+    <t>Wajib diisi menggunakan ID Tipe yang ada di sheet Data Tipe Messenger</t>
+  </si>
+  <si>
+    <t>Kode Kegunaan</t>
+  </si>
+  <si>
+    <t>Kegunaan</t>
+  </si>
+  <si>
+    <t>Kode Tipe Telepon</t>
+  </si>
+  <si>
+    <t>Tipe Telepon</t>
+  </si>
+  <si>
+    <t>Kode Messenger</t>
   </si>
 </sst>
 </file>
@@ -313,7 +331,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -338,6 +355,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,9 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -723,60 +739,60 @@
         <v>30</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="119" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="7" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -798,10 +814,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -822,10 +838,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -847,11 +863,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>56</v>
+      <c r="B1" s="13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1009,14 +1025,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>58</v>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3588,6 +3604,79 @@
       <c r="A515" s="2"/>
       <c r="B515" s="2"/>
       <c r="C515" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBA1FB6-5E08-6145-84E4-2646D0B2C23C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF57B37-231F-E242-BE7F-BC47CE65C85C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2634A6-8DE1-604D-A2E2-77E93BC9C10D}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3598,7 +3687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3615,46 +3704,46 @@
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>60</v>
+      <c r="G2" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3703,13 +3792,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3726,6 +3815,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625"/>
   </cols>
   <sheetData>
@@ -3734,24 +3824,24 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>47</v>
+      <c r="B2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3767,6 +3857,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3775,339 +3866,339 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
+      <c r="B2" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D3" s="10"/>
-      <c r="F3" s="12"/>
+      <c r="D3" s="9"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D4" s="10"/>
-      <c r="F4" s="12"/>
+      <c r="D4" s="9"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D5" s="10"/>
-      <c r="F5" s="12"/>
+      <c r="D5" s="9"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D6" s="10"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="9"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D7" s="10"/>
-      <c r="F7" s="12"/>
+      <c r="D7" s="9"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D8" s="10"/>
-      <c r="F8" s="12"/>
+      <c r="D8" s="9"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="10"/>
-      <c r="F9" s="12"/>
+      <c r="D9" s="9"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D10" s="10"/>
-      <c r="F10" s="12"/>
+      <c r="D10" s="9"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D11" s="10"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="9"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D12" s="10"/>
-      <c r="F12" s="12"/>
+      <c r="D12" s="9"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D13" s="10"/>
-      <c r="F13" s="12"/>
+      <c r="D13" s="9"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D14" s="10"/>
-      <c r="F14" s="12"/>
+      <c r="D14" s="9"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D15" s="10"/>
-      <c r="F15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D16" s="10"/>
-      <c r="F16" s="12"/>
+      <c r="D16" s="9"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D17" s="10"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="9"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D18" s="10"/>
-      <c r="F18" s="12"/>
+      <c r="D18" s="9"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D19" s="10"/>
-      <c r="F19" s="12"/>
+      <c r="D19" s="9"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D20" s="10"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="9"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D21" s="10"/>
-      <c r="F21" s="12"/>
+      <c r="D21" s="9"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D22" s="10"/>
-      <c r="F22" s="12"/>
+      <c r="D22" s="9"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D23" s="10"/>
-      <c r="F23" s="12"/>
+      <c r="D23" s="9"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D24" s="10"/>
-      <c r="F24" s="12"/>
+      <c r="D24" s="9"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D25" s="10"/>
-      <c r="F25" s="12"/>
+      <c r="D25" s="9"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D26" s="10"/>
-      <c r="F26" s="12"/>
+      <c r="D26" s="9"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D27" s="10"/>
-      <c r="F27" s="12"/>
+      <c r="D27" s="9"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D28" s="10"/>
-      <c r="F28" s="12"/>
+      <c r="D28" s="9"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D29" s="10"/>
-      <c r="F29" s="12"/>
+      <c r="D29" s="9"/>
+      <c r="F29" s="11"/>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D30" s="10"/>
-      <c r="F30" s="12"/>
+      <c r="D30" s="9"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D31" s="10"/>
-      <c r="F31" s="12"/>
+      <c r="D31" s="9"/>
+      <c r="F31" s="11"/>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D32" s="10"/>
-      <c r="F32" s="12"/>
+      <c r="D32" s="9"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D33" s="10"/>
-      <c r="F33" s="12"/>
+      <c r="D33" s="9"/>
+      <c r="F33" s="11"/>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D34" s="10"/>
-      <c r="F34" s="12"/>
+      <c r="D34" s="9"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="10"/>
-      <c r="F35" s="12"/>
+      <c r="D35" s="9"/>
+      <c r="F35" s="11"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D36" s="10"/>
-      <c r="F36" s="12"/>
+      <c r="D36" s="9"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D37" s="10"/>
-      <c r="F37" s="12"/>
+      <c r="D37" s="9"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D38" s="10"/>
-      <c r="F38" s="12"/>
+      <c r="D38" s="9"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D39" s="10"/>
-      <c r="F39" s="12"/>
+      <c r="D39" s="9"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D40" s="10"/>
-      <c r="F40" s="12"/>
+      <c r="D40" s="9"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D41" s="10"/>
-      <c r="F41" s="12"/>
+      <c r="D41" s="9"/>
+      <c r="F41" s="11"/>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D42" s="10"/>
-      <c r="F42" s="12"/>
+      <c r="D42" s="9"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D43" s="10"/>
-      <c r="F43" s="12"/>
+      <c r="D43" s="9"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D44" s="10"/>
-      <c r="F44" s="12"/>
+      <c r="D44" s="9"/>
+      <c r="F44" s="11"/>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D45" s="10"/>
-      <c r="F45" s="12"/>
+      <c r="D45" s="9"/>
+      <c r="F45" s="11"/>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D46" s="10"/>
-      <c r="F46" s="12"/>
+      <c r="D46" s="9"/>
+      <c r="F46" s="11"/>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D47" s="10"/>
-      <c r="F47" s="12"/>
+      <c r="D47" s="9"/>
+      <c r="F47" s="11"/>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D48" s="10"/>
-      <c r="F48" s="12"/>
+      <c r="D48" s="9"/>
+      <c r="F48" s="11"/>
     </row>
     <row r="49" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
-      <c r="F49" s="12"/>
+      <c r="D49" s="9"/>
+      <c r="F49" s="11"/>
     </row>
     <row r="50" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D50" s="10"/>
-      <c r="F50" s="12"/>
+      <c r="D50" s="9"/>
+      <c r="F50" s="11"/>
     </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D51" s="10"/>
-      <c r="F51" s="12"/>
+      <c r="D51" s="9"/>
+      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D52" s="10"/>
-      <c r="F52" s="12"/>
+      <c r="D52" s="9"/>
+      <c r="F52" s="11"/>
     </row>
     <row r="53" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D53" s="10"/>
-      <c r="F53" s="12"/>
+      <c r="D53" s="9"/>
+      <c r="F53" s="11"/>
     </row>
     <row r="54" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D54" s="10"/>
-      <c r="F54" s="12"/>
+      <c r="D54" s="9"/>
+      <c r="F54" s="11"/>
     </row>
     <row r="55" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D55" s="10"/>
-      <c r="F55" s="12"/>
+      <c r="D55" s="9"/>
+      <c r="F55" s="11"/>
     </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D56" s="10"/>
-      <c r="F56" s="12"/>
+      <c r="D56" s="9"/>
+      <c r="F56" s="11"/>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D57" s="10"/>
-      <c r="F57" s="12"/>
+      <c r="D57" s="9"/>
+      <c r="F57" s="11"/>
     </row>
     <row r="58" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D58" s="10"/>
-      <c r="F58" s="12"/>
+      <c r="D58" s="9"/>
+      <c r="F58" s="11"/>
     </row>
     <row r="59" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D59" s="10"/>
-      <c r="F59" s="12"/>
+      <c r="D59" s="9"/>
+      <c r="F59" s="11"/>
     </row>
     <row r="60" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D60" s="10"/>
-      <c r="F60" s="12"/>
+      <c r="D60" s="9"/>
+      <c r="F60" s="11"/>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D61" s="10"/>
-      <c r="F61" s="12"/>
+      <c r="D61" s="9"/>
+      <c r="F61" s="11"/>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D62" s="10"/>
-      <c r="F62" s="12"/>
+      <c r="D62" s="9"/>
+      <c r="F62" s="11"/>
     </row>
     <row r="63" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D63" s="10"/>
-      <c r="F63" s="12"/>
+      <c r="D63" s="9"/>
+      <c r="F63" s="11"/>
     </row>
     <row r="64" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D64" s="10"/>
-      <c r="F64" s="12"/>
+      <c r="D64" s="9"/>
+      <c r="F64" s="11"/>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D65" s="10"/>
-      <c r="F65" s="12"/>
+      <c r="D65" s="9"/>
+      <c r="F65" s="11"/>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D66" s="10"/>
-      <c r="F66" s="12"/>
+      <c r="D66" s="9"/>
+      <c r="F66" s="11"/>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D67" s="10"/>
-      <c r="F67" s="12"/>
+      <c r="D67" s="9"/>
+      <c r="F67" s="11"/>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D68" s="10"/>
-      <c r="F68" s="12"/>
+      <c r="D68" s="9"/>
+      <c r="F68" s="11"/>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D69" s="10"/>
-      <c r="F69" s="12"/>
+      <c r="D69" s="9"/>
+      <c r="F69" s="11"/>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D70" s="10"/>
-      <c r="F70" s="12"/>
+      <c r="D70" s="9"/>
+      <c r="F70" s="11"/>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D71" s="10"/>
-      <c r="F71" s="12"/>
+      <c r="D71" s="9"/>
+      <c r="F71" s="11"/>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D72" s="10"/>
-      <c r="F72" s="12"/>
+      <c r="D72" s="9"/>
+      <c r="F72" s="11"/>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D73" s="10"/>
-      <c r="F73" s="12"/>
+      <c r="D73" s="9"/>
+      <c r="F73" s="11"/>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D74" s="10"/>
-      <c r="F74" s="12"/>
+      <c r="D74" s="9"/>
+      <c r="F74" s="11"/>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D75" s="10"/>
-      <c r="F75" s="12"/>
+      <c r="D75" s="9"/>
+      <c r="F75" s="11"/>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D76" s="10"/>
-      <c r="F76" s="12"/>
+      <c r="D76" s="9"/>
+      <c r="F76" s="11"/>
     </row>
     <row r="77" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D77" s="10"/>
-      <c r="F77" s="12"/>
+      <c r="D77" s="9"/>
+      <c r="F77" s="11"/>
     </row>
     <row r="78" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D78" s="10"/>
-      <c r="F78" s="12"/>
+      <c r="D78" s="9"/>
+      <c r="F78" s="11"/>
     </row>
     <row r="79" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D79" s="10"/>
-      <c r="F79" s="12"/>
+      <c r="D79" s="9"/>
+      <c r="F79" s="11"/>
     </row>
     <row r="80" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D80" s="10"/>
-      <c r="F80" s="12"/>
+      <c r="D80" s="9"/>
+      <c r="F80" s="11"/>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D81" s="10"/>
-      <c r="F81" s="12"/>
+      <c r="D81" s="9"/>
+      <c r="F81" s="11"/>
     </row>
     <row r="82" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D82" s="10"/>
-      <c r="F82" s="12"/>
+      <c r="D82" s="9"/>
+      <c r="F82" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -4123,6 +4214,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4131,25 +4223,28 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>52</v>
+      <c r="B2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="10"/>
+      <c r="B3" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4168,10 +4263,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4192,11 +4287,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>55</v>
+      <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -4216,10 +4311,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove field password in Import Excel
</commit_message>
<xml_diff>
--- a/public/template/Template_Input_Staff.xlsx
+++ b/public/template/Template_Input_Staff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadmukhtar/Projects/rpc-be/public/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E380AA-1315-E64C-9AC7-645230C9F365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EBE5D4-5E0C-A848-AC82-34E64E599F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detail" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>Wajib diisi berdasarkan nomor urut dan tidak boleh duplikat</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>Nama Kabupaten / Kota</t>
-  </si>
-  <si>
-    <t>Password</t>
   </si>
   <si>
     <t>Diisi menggunakan ID dari sheet Data Grup Keamanan</t>
@@ -666,9 +663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -716,7 +711,7 @@
         <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>17</v>
@@ -757,9 +752,7 @@
       <c r="U1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
@@ -784,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>5</v>
@@ -815,10 +808,10 @@
         <v>8</v>
       </c>
       <c r="S2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="T2" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3672,10 +3665,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3697,10 +3690,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -3721,10 +3714,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -3792,7 +3785,7 @@
         <v>31</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3873,13 +3866,13 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
@@ -3887,10 +3880,10 @@
         <v>30</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -3915,7 +3908,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>45</v>
@@ -3926,7 +3919,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -4272,13 +4265,13 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
@@ -4286,10 +4279,10 @@
         <v>30</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4304,7 +4297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C7F05F-52C1-FB4A-93FC-482C86C08DEF}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4317,7 +4310,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>